<commit_message>
Fixing water issues in ecoinvent database. Still need to fix water for regioinvent as a whole.
</commit_message>
<xml_diff>
--- a/Data/ei_iw_geo_mapping.xlsx
+++ b/Data/ei_iw_geo_mapping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\11max\PycharmProjects\Regioinvent\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC9BB80-2F99-427E-A789-40DF260792F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC267262-51DF-4B00-B576-A3A075C4065E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{91CF7D30-F020-4F0F-B7E1-F06EBC5EAD55}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1550" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1555" uniqueCount="316">
   <si>
     <t>AE</t>
   </si>
@@ -1355,10 +1355,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9C8BF03-FE90-413A-BA68-8F3BBE4EDF18}">
-  <dimension ref="A1:E310"/>
+  <dimension ref="A1:E311"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5428,228 +5428,228 @@
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>236</v>
+        <v>311</v>
       </c>
       <c r="B240" t="s">
-        <v>236</v>
+        <v>311</v>
       </c>
       <c r="C240" t="s">
-        <v>247</v>
+        <v>311</v>
       </c>
       <c r="D240" t="s">
-        <v>236</v>
+        <v>311</v>
       </c>
       <c r="E240" t="s">
-        <v>236</v>
+        <v>311</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B241" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C241" t="s">
-        <v>237</v>
+        <v>247</v>
       </c>
       <c r="D241" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E241" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B242" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C242" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D242" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E242" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B243" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C243" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D243" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E243" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B244" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C244" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D244" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E244" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B245" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C245" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D245" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E245" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B246" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C246" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D246" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E246" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B247" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C247" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D247" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E247" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B248" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C248" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D248" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E248" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B249" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C249" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="D249" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E249" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B250" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C250" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D250" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E250" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B251" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C251" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D251" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E251" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B252" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C252" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D252" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E252" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B253" t="s">
         <v>248</v>
@@ -5666,7 +5666,7 @@
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B254" t="s">
         <v>248</v>
@@ -5683,7 +5683,7 @@
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B255" t="s">
         <v>248</v>
@@ -5700,534 +5700,534 @@
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B256" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C256" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D256" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="E256" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B257" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C257" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="D257" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="E257" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B258" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C258" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="D258" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="E258" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B259" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C259" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D259" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E259" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B260" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C260" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D260" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="E260" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B261" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C261" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D261" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="E261" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B262" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C262" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D262" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E262" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B263" t="s">
-        <v>248</v>
+        <v>258</v>
       </c>
       <c r="C263" t="s">
-        <v>248</v>
+        <v>258</v>
       </c>
       <c r="D263" t="s">
-        <v>248</v>
+        <v>258</v>
       </c>
       <c r="E263" t="s">
-        <v>248</v>
+        <v>258</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
-        <v>310</v>
+        <v>259</v>
       </c>
       <c r="B264" t="s">
-        <v>310</v>
+        <v>248</v>
       </c>
       <c r="C264" t="s">
-        <v>309</v>
+        <v>248</v>
       </c>
       <c r="D264" t="s">
-        <v>309</v>
+        <v>248</v>
       </c>
       <c r="E264" t="s">
-        <v>309</v>
+        <v>248</v>
       </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
-        <v>260</v>
+        <v>310</v>
       </c>
       <c r="B265" t="s">
-        <v>260</v>
+        <v>310</v>
       </c>
       <c r="C265" t="s">
-        <v>247</v>
+        <v>309</v>
       </c>
       <c r="D265" t="s">
-        <v>260</v>
+        <v>309</v>
       </c>
       <c r="E265" t="s">
-        <v>260</v>
+        <v>309</v>
       </c>
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B266" t="s">
-        <v>247</v>
+        <v>260</v>
       </c>
       <c r="C266" t="s">
         <v>247</v>
       </c>
       <c r="D266" t="s">
-        <v>247</v>
+        <v>260</v>
       </c>
       <c r="E266" t="s">
-        <v>247</v>
+        <v>260</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B267" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="C267" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="D267" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="E267" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B268" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C268" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D268" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E268" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B269" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C269" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D269" t="s">
-        <v>247</v>
+        <v>263</v>
       </c>
       <c r="E269" t="s">
-        <v>247</v>
+        <v>263</v>
       </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B270" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C270" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D270" t="s">
-        <v>265</v>
+        <v>247</v>
       </c>
       <c r="E270" t="s">
-        <v>265</v>
+        <v>247</v>
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B271" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C271" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D271" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E271" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B272" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C272" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D272" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E272" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B273" t="s">
-        <v>246</v>
+        <v>267</v>
       </c>
       <c r="C273" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D273" t="s">
-        <v>246</v>
+        <v>267</v>
       </c>
       <c r="E273" t="s">
-        <v>246</v>
+        <v>267</v>
       </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B274" t="s">
-        <v>269</v>
+        <v>246</v>
       </c>
       <c r="C274" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D274" t="s">
-        <v>269</v>
+        <v>246</v>
       </c>
       <c r="E274" t="s">
-        <v>269</v>
+        <v>246</v>
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B275" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C275" t="s">
-        <v>247</v>
+        <v>269</v>
       </c>
       <c r="D275" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E275" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B276" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C276" t="s">
-        <v>271</v>
+        <v>247</v>
       </c>
       <c r="D276" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E276" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B277" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C277" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D277" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E277" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B278" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C278" t="s">
-        <v>247</v>
+        <v>272</v>
       </c>
       <c r="D278" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E278" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B279" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C279" t="s">
         <v>247</v>
       </c>
       <c r="D279" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E279" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B280" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C280" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
       <c r="D280" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E280" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B281" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C281" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D281" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E281" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B282" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C282" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D282" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E282" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B283" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C283" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D283" t="s">
-        <v>247</v>
+        <v>277</v>
       </c>
       <c r="E283" t="s">
-        <v>247</v>
+        <v>277</v>
       </c>
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B284" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C284" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D284" t="s">
-        <v>279</v>
+        <v>247</v>
       </c>
       <c r="E284" t="s">
-        <v>279</v>
+        <v>247</v>
       </c>
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B285" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C285" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D285" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E285" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B286" t="s">
-        <v>248</v>
+        <v>280</v>
       </c>
       <c r="C286" t="s">
-        <v>248</v>
+        <v>280</v>
       </c>
       <c r="D286" t="s">
-        <v>248</v>
+        <v>280</v>
       </c>
       <c r="E286" t="s">
-        <v>248</v>
+        <v>280</v>
       </c>
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B287" t="s">
         <v>248</v>
@@ -6244,58 +6244,58 @@
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B288" t="s">
-        <v>311</v>
+        <v>248</v>
       </c>
       <c r="C288" t="s">
-        <v>311</v>
+        <v>248</v>
       </c>
       <c r="D288" t="s">
-        <v>311</v>
+        <v>248</v>
       </c>
       <c r="E288" t="s">
-        <v>311</v>
+        <v>248</v>
       </c>
     </row>
     <row r="289" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B289" t="s">
-        <v>247</v>
+        <v>311</v>
       </c>
       <c r="C289" t="s">
-        <v>247</v>
+        <v>311</v>
       </c>
       <c r="D289" t="s">
-        <v>247</v>
+        <v>311</v>
       </c>
       <c r="E289" t="s">
-        <v>247</v>
+        <v>311</v>
       </c>
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B290" t="s">
-        <v>285</v>
+        <v>247</v>
       </c>
       <c r="C290" t="s">
-        <v>285</v>
+        <v>247</v>
       </c>
       <c r="D290" t="s">
-        <v>285</v>
+        <v>247</v>
       </c>
       <c r="E290" t="s">
-        <v>285</v>
+        <v>247</v>
       </c>
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B291" t="s">
         <v>285</v>
@@ -6312,7 +6312,7 @@
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B292" t="s">
         <v>285</v>
@@ -6329,7 +6329,7 @@
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B293" t="s">
         <v>285</v>
@@ -6346,7 +6346,7 @@
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B294" t="s">
         <v>285</v>
@@ -6363,41 +6363,41 @@
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B295" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="C295" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="D295" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="E295" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B296" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="C296" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="D296" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="E296" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
     </row>
     <row r="297" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B297" t="s">
         <v>285</v>
@@ -6414,7 +6414,7 @@
     </row>
     <row r="298" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B298" t="s">
         <v>285</v>
@@ -6431,7 +6431,7 @@
     </row>
     <row r="299" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B299" t="s">
         <v>285</v>
@@ -6448,109 +6448,109 @@
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B300" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="C300" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="D300" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="E300" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
     </row>
     <row r="301" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B301" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C301" t="s">
-        <v>247</v>
+        <v>296</v>
       </c>
       <c r="D301" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E301" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B302" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C302" t="s">
-        <v>298</v>
+        <v>247</v>
       </c>
       <c r="D302" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E302" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B303" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C303" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D303" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E303" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B304" t="s">
-        <v>285</v>
+        <v>299</v>
       </c>
       <c r="C304" t="s">
-        <v>285</v>
+        <v>299</v>
       </c>
       <c r="D304" t="s">
-        <v>285</v>
+        <v>299</v>
       </c>
       <c r="E304" t="s">
-        <v>285</v>
+        <v>299</v>
       </c>
     </row>
     <row r="305" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B305" t="s">
-        <v>248</v>
+        <v>285</v>
       </c>
       <c r="C305" t="s">
-        <v>248</v>
+        <v>285</v>
       </c>
       <c r="D305" t="s">
-        <v>248</v>
+        <v>285</v>
       </c>
       <c r="E305" t="s">
-        <v>248</v>
+        <v>285</v>
       </c>
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B306" t="s">
         <v>248</v>
@@ -6567,69 +6567,86 @@
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B307" t="s">
-        <v>303</v>
+        <v>248</v>
       </c>
       <c r="C307" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D307" t="s">
-        <v>303</v>
+        <v>248</v>
       </c>
       <c r="E307" t="s">
-        <v>303</v>
+        <v>248</v>
       </c>
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B308" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C308" t="s">
-        <v>304</v>
+        <v>247</v>
       </c>
       <c r="D308" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E308" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="309" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B309" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C309" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D309" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E309" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
+        <v>305</v>
+      </c>
+      <c r="B310" t="s">
+        <v>305</v>
+      </c>
+      <c r="C310" t="s">
+        <v>305</v>
+      </c>
+      <c r="D310" t="s">
+        <v>305</v>
+      </c>
+      <c r="E310" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="311" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A311" t="s">
         <v>306</v>
       </c>
-      <c r="B310" t="s">
+      <c r="B311" t="s">
         <v>306</v>
       </c>
-      <c r="C310" t="s">
+      <c r="C311" t="s">
         <v>306</v>
       </c>
-      <c r="D310" t="s">
+      <c r="D311" t="s">
         <v>306</v>
       </c>
-      <c r="E310" t="s">
+      <c r="E311" t="s">
         <v>306</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Working with the new format of the UN COMTRADE data + created water technosphere processes are now regionalized as well (electricity, heat and waste)
</commit_message>
<xml_diff>
--- a/Data/ei_iw_geo_mapping.xlsx
+++ b/Data/ei_iw_geo_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\11max\PycharmProjects\Regioinvent\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93059AF5-79A6-4314-8FF1-84FDFB22EA72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0EC74D4-4000-4CC3-ABC1-78A70F42A8BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{91CF7D30-F020-4F0F-B7E1-F06EBC5EAD55}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1685" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1690" uniqueCount="343">
   <si>
     <t>AE</t>
   </si>
@@ -1062,6 +1062,9 @@
   </si>
   <si>
     <t>VC</t>
+  </si>
+  <si>
+    <t>WS</t>
   </si>
 </sst>
 </file>
@@ -1433,10 +1436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9C8BF03-FE90-413A-BA68-8F3BBE4EDF18}">
-  <dimension ref="A1:E337"/>
+  <dimension ref="A1:E338"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A311" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B319" sqref="B319"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7087,86 +7090,103 @@
     </row>
     <row r="333" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
-        <v>302</v>
+        <v>342</v>
       </c>
       <c r="B333" t="s">
-        <v>248</v>
+        <v>342</v>
       </c>
       <c r="C333" t="s">
-        <v>248</v>
+        <v>311</v>
       </c>
       <c r="D333" t="s">
-        <v>248</v>
+        <v>311</v>
       </c>
       <c r="E333" t="s">
-        <v>248</v>
+        <v>311</v>
       </c>
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B334" t="s">
-        <v>303</v>
+        <v>248</v>
       </c>
       <c r="C334" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D334" t="s">
-        <v>303</v>
+        <v>248</v>
       </c>
       <c r="E334" t="s">
-        <v>303</v>
+        <v>248</v>
       </c>
     </row>
     <row r="335" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B335" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C335" t="s">
-        <v>304</v>
+        <v>247</v>
       </c>
       <c r="D335" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E335" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="336" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B336" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C336" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D336" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E336" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="337" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
+        <v>305</v>
+      </c>
+      <c r="B337" t="s">
+        <v>305</v>
+      </c>
+      <c r="C337" t="s">
+        <v>305</v>
+      </c>
+      <c r="D337" t="s">
+        <v>305</v>
+      </c>
+      <c r="E337" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="338" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A338" t="s">
         <v>306</v>
       </c>
-      <c r="B337" t="s">
+      <c r="B338" t="s">
         <v>306</v>
       </c>
-      <c r="C337" t="s">
+      <c r="C338" t="s">
         <v>306</v>
       </c>
-      <c r="D337" t="s">
+      <c r="D338" t="s">
         <v>306</v>
       </c>
-      <c r="E337" t="s">
+      <c r="E338" t="s">
         <v>306</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Small corrections in mapping of land regionalized flows.
</commit_message>
<xml_diff>
--- a/Data/ei_iw_geo_mapping.xlsx
+++ b/Data/ei_iw_geo_mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\11max\PycharmProjects\Regioinvent\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0EC74D4-4000-4CC3-ABC1-78A70F42A8BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E95123-13AF-42DC-AEA2-4B38B76D726D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{91CF7D30-F020-4F0F-B7E1-F06EBC5EAD55}"/>
+    <workbookView xWindow="28695" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{91CF7D30-F020-4F0F-B7E1-F06EBC5EAD55}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1438,9 +1438,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9C8BF03-FE90-413A-BA68-8F3BBE4EDF18}">
   <dimension ref="A1:E338"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A311" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B319" sqref="B319"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -1486,10 +1484,10 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>247</v>
+        <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>247</v>
+        <v>0</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
@@ -1520,7 +1518,7 @@
         <v>317</v>
       </c>
       <c r="C5" t="s">
-        <v>252</v>
+        <v>317</v>
       </c>
       <c r="D5" t="s">
         <v>317</v>
@@ -1724,7 +1722,7 @@
         <v>319</v>
       </c>
       <c r="C17" t="s">
-        <v>246</v>
+        <v>319</v>
       </c>
       <c r="D17" t="s">
         <v>319</v>
@@ -1775,7 +1773,7 @@
         <v>320</v>
       </c>
       <c r="C20" t="s">
-        <v>246</v>
+        <v>320</v>
       </c>
       <c r="D20" t="s">
         <v>320</v>
@@ -2438,7 +2436,7 @@
         <v>322</v>
       </c>
       <c r="C59" t="s">
-        <v>252</v>
+        <v>322</v>
       </c>
       <c r="D59" t="s">
         <v>322</v>
@@ -2710,7 +2708,7 @@
         <v>323</v>
       </c>
       <c r="C75" t="s">
-        <v>246</v>
+        <v>323</v>
       </c>
       <c r="D75" t="s">
         <v>323</v>
@@ -3543,7 +3541,7 @@
         <v>252</v>
       </c>
       <c r="C124" t="s">
-        <v>252</v>
+        <v>113</v>
       </c>
       <c r="D124" t="s">
         <v>252</v>
@@ -3560,7 +3558,7 @@
         <v>114</v>
       </c>
       <c r="C125" t="s">
-        <v>248</v>
+        <v>114</v>
       </c>
       <c r="D125" t="s">
         <v>114</v>
@@ -3713,7 +3711,7 @@
         <v>123</v>
       </c>
       <c r="C134" t="s">
-        <v>246</v>
+        <v>123</v>
       </c>
       <c r="D134" t="s">
         <v>123</v>
@@ -3883,7 +3881,7 @@
         <v>324</v>
       </c>
       <c r="C144" t="s">
-        <v>311</v>
+        <v>324</v>
       </c>
       <c r="D144" t="s">
         <v>324</v>
@@ -4019,7 +4017,7 @@
         <v>339</v>
       </c>
       <c r="C152" t="s">
-        <v>246</v>
+        <v>339</v>
       </c>
       <c r="D152" t="s">
         <v>339</v>
@@ -4070,7 +4068,7 @@
         <v>325</v>
       </c>
       <c r="C155" t="s">
-        <v>252</v>
+        <v>325</v>
       </c>
       <c r="D155" t="s">
         <v>325</v>
@@ -4084,7 +4082,7 @@
         <v>140</v>
       </c>
       <c r="B156" t="s">
-        <v>70</v>
+        <v>140</v>
       </c>
       <c r="C156" t="s">
         <v>140</v>
@@ -4325,7 +4323,7 @@
         <v>154</v>
       </c>
       <c r="C170" t="s">
-        <v>247</v>
+        <v>154</v>
       </c>
       <c r="D170" t="s">
         <v>154</v>
@@ -5039,7 +5037,7 @@
         <v>196</v>
       </c>
       <c r="C212" t="s">
-        <v>248</v>
+        <v>196</v>
       </c>
       <c r="D212" t="s">
         <v>196</v>
@@ -5090,7 +5088,7 @@
         <v>199</v>
       </c>
       <c r="C215" t="s">
-        <v>247</v>
+        <v>199</v>
       </c>
       <c r="D215" t="s">
         <v>199</v>
@@ -5209,7 +5207,7 @@
         <v>206</v>
       </c>
       <c r="C222" t="s">
-        <v>247</v>
+        <v>206</v>
       </c>
       <c r="D222" t="s">
         <v>206</v>
@@ -5243,7 +5241,7 @@
         <v>326</v>
       </c>
       <c r="C224" t="s">
-        <v>247</v>
+        <v>326</v>
       </c>
       <c r="D224" t="s">
         <v>326</v>
@@ -5260,7 +5258,7 @@
         <v>208</v>
       </c>
       <c r="C225" t="s">
-        <v>247</v>
+        <v>208</v>
       </c>
       <c r="D225" t="s">
         <v>208</v>
@@ -5277,7 +5275,7 @@
         <v>340</v>
       </c>
       <c r="C226" t="s">
-        <v>252</v>
+        <v>340</v>
       </c>
       <c r="D226" t="s">
         <v>340</v>
@@ -5311,7 +5309,7 @@
         <v>327</v>
       </c>
       <c r="C228" t="s">
-        <v>246</v>
+        <v>327</v>
       </c>
       <c r="D228" t="s">
         <v>327</v>
@@ -5379,7 +5377,7 @@
         <v>213</v>
       </c>
       <c r="C232" t="s">
-        <v>246</v>
+        <v>213</v>
       </c>
       <c r="D232" t="s">
         <v>213</v>
@@ -5481,7 +5479,7 @@
         <v>328</v>
       </c>
       <c r="C238" t="s">
-        <v>246</v>
+        <v>328</v>
       </c>
       <c r="D238" t="s">
         <v>328</v>
@@ -5532,7 +5530,7 @@
         <v>329</v>
       </c>
       <c r="C241" t="s">
-        <v>246</v>
+        <v>329</v>
       </c>
       <c r="D241" t="s">
         <v>329</v>
@@ -5549,7 +5547,7 @@
         <v>330</v>
       </c>
       <c r="C242" t="s">
-        <v>252</v>
+        <v>330</v>
       </c>
       <c r="D242" t="s">
         <v>330</v>
@@ -5566,7 +5564,7 @@
         <v>221</v>
       </c>
       <c r="C243" t="s">
-        <v>248</v>
+        <v>221</v>
       </c>
       <c r="D243" t="s">
         <v>221</v>
@@ -5617,7 +5615,7 @@
         <v>331</v>
       </c>
       <c r="C246" t="s">
-        <v>246</v>
+        <v>331</v>
       </c>
       <c r="D246" t="s">
         <v>331</v>
@@ -5855,7 +5853,7 @@
         <v>236</v>
       </c>
       <c r="C260" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="D260" t="s">
         <v>236</v>
@@ -6025,7 +6023,7 @@
         <v>245</v>
       </c>
       <c r="C270" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D270" t="s">
         <v>245</v>
@@ -6297,7 +6295,7 @@
         <v>260</v>
       </c>
       <c r="C286" t="s">
-        <v>247</v>
+        <v>260</v>
       </c>
       <c r="D286" t="s">
         <v>260</v>
@@ -6331,7 +6329,7 @@
         <v>247</v>
       </c>
       <c r="C288" t="s">
-        <v>247</v>
+        <v>333</v>
       </c>
       <c r="D288" t="s">
         <v>333</v>
@@ -6450,7 +6448,7 @@
         <v>334</v>
       </c>
       <c r="C295" t="s">
-        <v>252</v>
+        <v>334</v>
       </c>
       <c r="D295" t="s">
         <v>334</v>
@@ -6501,7 +6499,7 @@
         <v>270</v>
       </c>
       <c r="C298" t="s">
-        <v>247</v>
+        <v>270</v>
       </c>
       <c r="D298" t="s">
         <v>270</v>
@@ -6518,7 +6516,7 @@
         <v>335</v>
       </c>
       <c r="C299" t="s">
-        <v>246</v>
+        <v>335</v>
       </c>
       <c r="D299" t="s">
         <v>335</v>
@@ -6569,7 +6567,7 @@
         <v>273</v>
       </c>
       <c r="C302" t="s">
-        <v>247</v>
+        <v>273</v>
       </c>
       <c r="D302" t="s">
         <v>273</v>
@@ -6586,7 +6584,7 @@
         <v>336</v>
       </c>
       <c r="C303" t="s">
-        <v>247</v>
+        <v>336</v>
       </c>
       <c r="D303" t="s">
         <v>336</v>
@@ -6756,7 +6754,7 @@
         <v>337</v>
       </c>
       <c r="C313" t="s">
-        <v>246</v>
+        <v>337</v>
       </c>
       <c r="D313" t="s">
         <v>337</v>
@@ -6994,7 +6992,7 @@
         <v>297</v>
       </c>
       <c r="C327" t="s">
-        <v>247</v>
+        <v>297</v>
       </c>
       <c r="D327" t="s">
         <v>297</v>
@@ -7096,13 +7094,13 @@
         <v>342</v>
       </c>
       <c r="C333" t="s">
-        <v>311</v>
+        <v>342</v>
       </c>
       <c r="D333" t="s">
-        <v>311</v>
+        <v>247</v>
       </c>
       <c r="E333" t="s">
-        <v>311</v>
+        <v>247</v>
       </c>
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.3">
@@ -7130,7 +7128,7 @@
         <v>303</v>
       </c>
       <c r="C335" t="s">
-        <v>247</v>
+        <v>303</v>
       </c>
       <c r="D335" t="s">
         <v>303</v>

</xml_diff>